<commit_message>
Added next game probability deltas
</commit_message>
<xml_diff>
--- a/Probabilities.xlsx
+++ b/Probabilities.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="25">
   <si>
     <t>Team</t>
   </si>
@@ -35,6 +35,15 @@
     <t>mi</t>
   </si>
   <si>
+    <t>37.5%</t>
+  </si>
+  <si>
+    <t>87.5%</t>
+  </si>
+  <si>
+    <t>100.0%</t>
+  </si>
+  <si>
     <t>dc</t>
   </si>
   <si>
@@ -44,6 +53,12 @@
     <t>kkr</t>
   </si>
   <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>75.0%</t>
+  </si>
+  <si>
     <t>srh</t>
   </si>
   <si>
@@ -53,7 +68,28 @@
     <t>rr</t>
   </si>
   <si>
+    <t>25.0%</t>
+  </si>
+  <si>
     <t>kxip</t>
+  </si>
+  <si>
+    <t>if dc wins</t>
+  </si>
+  <si>
+    <t>-25.0%</t>
+  </si>
+  <si>
+    <t>-50.0%</t>
+  </si>
+  <si>
+    <t>-37.5%</t>
+  </si>
+  <si>
+    <t>if rr wins</t>
+  </si>
+  <si>
+    <t>-12.5%</t>
   </si>
 </sst>
 </file>
@@ -400,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,9 +444,11 @@
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,140 +465,436 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
-        <v>37.5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>87.5</v>
-      </c>
-      <c r="D2" s="3">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>37.5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>87.5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>100</v>
-      </c>
-      <c r="E3" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
-        <v>37.5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>87.5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
-        <v>37.5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added addendum image,fixed issue in delta calculation
</commit_message>
<xml_diff>
--- a/Probabilities.xlsx
+++ b/Probabilities.xlsx
@@ -74,22 +74,22 @@
     <t>kxip</t>
   </si>
   <si>
-    <t>if dc wins</t>
+    <t>Change if dc wins</t>
+  </si>
+  <si>
+    <t>-12.5%</t>
+  </si>
+  <si>
+    <t>12.5%</t>
   </si>
   <si>
     <t>-25.0%</t>
   </si>
   <si>
-    <t>-50.0%</t>
+    <t>Change if rr wins</t>
   </si>
   <si>
     <t>-37.5%</t>
-  </si>
-  <si>
-    <t>if rr wins</t>
-  </si>
-  <si>
-    <t>-12.5%</t>
   </si>
 </sst>
 </file>
@@ -149,6 +149,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1108542</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>49750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Addendum.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7181850" y="190500"/>
+          <a:ext cx="6299667" cy="1573750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,9 +485,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,28 +692,28 @@
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -678,31 +721,31 @@
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -713,28 +756,28 @@
         <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -748,10 +791,10 @@
         <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -760,13 +803,13 @@
         <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -847,7 +890,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G19" t="s">
         <v>16</v>
@@ -862,7 +905,7 @@
         <v>12</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -899,6 +942,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>